<commit_message>
Updated excel file with top entries
</commit_message>
<xml_diff>
--- a/autolysis/metadata-template.xlsx
+++ b/autolysis/metadata-template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\site\gramener.com\viz\autolysis\autolysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satheesh\Desktop\autolysis\autolysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Source</t>
   </si>
   <si>
-    <t># ['name']</t>
-  </si>
-  <si>
     <t># ['source']</t>
   </si>
   <si>
@@ -55,12 +49,36 @@
   </si>
   <si>
     <t># ['columns'][*]['nunique']</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t># ['format']</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>#['rows']</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>#['columns'][*]['top']</t>
+  </si>
+  <si>
+    <t>Moments</t>
+  </si>
+  <si>
+    <t>#['columns'][*]['moments']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,6 +203,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -220,6 +255,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -396,56 +448,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>